<commit_message>
update sheet third column
</commit_message>
<xml_diff>
--- a/testSheet.xlsx
+++ b/testSheet.xlsx
@@ -12,18 +12,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Tiny; hamlet with 1d2 buildings remaining</t>
   </si>
   <si>
+    <t>1d2</t>
+  </si>
+  <si>
     <t>Small; village with 1d4+1 buildings remaining</t>
   </si>
   <si>
+    <t>1d4+1</t>
+  </si>
+  <si>
     <t>Medium; town with 1d6+2 buildings remaining</t>
   </si>
   <si>
+    <t>1d6+2</t>
+  </si>
+  <si>
     <t>Large; large town with 1d8+3 buildings remaining</t>
+  </si>
+  <si>
+    <t>1d8+3</t>
   </si>
   <si>
     <t>Religious, roll on Religious Ruins Table</t>
@@ -315,13 +327,19 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
         <v>2.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -329,7 +347,10 @@
         <v>3.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -337,7 +358,10 @@
         <v>4.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -360,7 +384,7 @@
         <v>1.0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">
@@ -368,7 +392,7 @@
         <v>2.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -376,7 +400,7 @@
         <v>3.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -384,7 +408,7 @@
         <v>4.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
@@ -392,7 +416,7 @@
         <v>5.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -400,7 +424,7 @@
         <v>6.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
@@ -408,7 +432,7 @@
         <v>7.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
@@ -416,7 +440,7 @@
         <v>8.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>